<commit_message>
Fix labor calendar feasibility validation error
Two-part fix for ValueError when planning horizon extends before forecast start:

1. Smart validation logic (integrated_model.py):
   - Distinguish weekday vs weekend missing dates
   - Weekdays (Mon-Fri) trigger errors (production should be available)
   - Weekends (Sat-Sun) issue warnings only (optional production)
   - Model already handles missing dates as zero capacity

2. Extended data coverage (generate_network_config.py):
   - Labor calendar now starts May 26 (7 days before forecast)
   - Covers 211 days instead of 204
   - Accounts for planning horizon buffer needed for route transit times

Resolves error: "Labor calendar missing entries for 2025-05-30, 2025-05-31, 2025-06-01"

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/examples/Network_Config.xlsx
+++ b/data/examples/Network_Config.xlsx
@@ -1120,7 +1120,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G205"/>
+  <dimension ref="A1:G212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45810</v>
+        <v>45803</v>
       </c>
       <c r="B2" t="n">
         <v>12</v>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45811</v>
+        <v>45804</v>
       </c>
       <c r="B3" t="n">
         <v>12</v>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45812</v>
+        <v>45805</v>
       </c>
       <c r="B4" t="n">
         <v>12</v>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45813</v>
+        <v>45806</v>
       </c>
       <c r="B5" t="n">
         <v>12</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45814</v>
+        <v>45807</v>
       </c>
       <c r="B6" t="n">
         <v>12</v>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45815</v>
+        <v>45808</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45816</v>
+        <v>45809</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -1318,10 +1318,10 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45817</v>
+        <v>45810</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
         <v>25</v>
@@ -1329,19 +1329,17 @@
       <c r="D9" t="n">
         <v>37.5</v>
       </c>
-      <c r="E9" t="n">
-        <v>40</v>
-      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45818</v>
+        <v>45811</v>
       </c>
       <c r="B10" t="n">
         <v>12</v>
@@ -1362,7 +1360,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45819</v>
+        <v>45812</v>
       </c>
       <c r="B11" t="n">
         <v>12</v>
@@ -1383,7 +1381,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45820</v>
+        <v>45813</v>
       </c>
       <c r="B12" t="n">
         <v>12</v>
@@ -1404,7 +1402,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45821</v>
+        <v>45814</v>
       </c>
       <c r="B13" t="n">
         <v>12</v>
@@ -1425,7 +1423,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45822</v>
+        <v>45815</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -1448,7 +1446,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45823</v>
+        <v>45816</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -1471,10 +1469,10 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45824</v>
+        <v>45817</v>
       </c>
       <c r="B16" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>25</v>
@@ -1482,17 +1480,19 @@
       <c r="D16" t="n">
         <v>37.5</v>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>40</v>
+      </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45825</v>
+        <v>45818</v>
       </c>
       <c r="B17" t="n">
         <v>12</v>
@@ -1513,7 +1513,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45826</v>
+        <v>45819</v>
       </c>
       <c r="B18" t="n">
         <v>12</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45827</v>
+        <v>45820</v>
       </c>
       <c r="B19" t="n">
         <v>12</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45828</v>
+        <v>45821</v>
       </c>
       <c r="B20" t="n">
         <v>12</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45829</v>
+        <v>45822</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45830</v>
+        <v>45823</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45831</v>
+        <v>45824</v>
       </c>
       <c r="B23" t="n">
         <v>12</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45832</v>
+        <v>45825</v>
       </c>
       <c r="B24" t="n">
         <v>12</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45833</v>
+        <v>45826</v>
       </c>
       <c r="B25" t="n">
         <v>12</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45834</v>
+        <v>45827</v>
       </c>
       <c r="B26" t="n">
         <v>12</v>
@@ -1706,7 +1706,7 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45835</v>
+        <v>45828</v>
       </c>
       <c r="B27" t="n">
         <v>12</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45836</v>
+        <v>45829</v>
       </c>
       <c r="B28" t="n">
         <v>0</v>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45837</v>
+        <v>45830</v>
       </c>
       <c r="B29" t="n">
         <v>0</v>
@@ -1773,7 +1773,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45838</v>
+        <v>45831</v>
       </c>
       <c r="B30" t="n">
         <v>12</v>
@@ -1794,7 +1794,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45839</v>
+        <v>45832</v>
       </c>
       <c r="B31" t="n">
         <v>12</v>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45840</v>
+        <v>45833</v>
       </c>
       <c r="B32" t="n">
         <v>12</v>
@@ -1836,7 +1836,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45841</v>
+        <v>45834</v>
       </c>
       <c r="B33" t="n">
         <v>12</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45842</v>
+        <v>45835</v>
       </c>
       <c r="B34" t="n">
         <v>12</v>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45843</v>
+        <v>45836</v>
       </c>
       <c r="B35" t="n">
         <v>0</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45844</v>
+        <v>45837</v>
       </c>
       <c r="B36" t="n">
         <v>0</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45845</v>
+        <v>45838</v>
       </c>
       <c r="B37" t="n">
         <v>12</v>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45846</v>
+        <v>45839</v>
       </c>
       <c r="B38" t="n">
         <v>12</v>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45847</v>
+        <v>45840</v>
       </c>
       <c r="B39" t="n">
         <v>12</v>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45848</v>
+        <v>45841</v>
       </c>
       <c r="B40" t="n">
         <v>12</v>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45849</v>
+        <v>45842</v>
       </c>
       <c r="B41" t="n">
         <v>12</v>
@@ -2029,7 +2029,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45850</v>
+        <v>45843</v>
       </c>
       <c r="B42" t="n">
         <v>0</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45851</v>
+        <v>45844</v>
       </c>
       <c r="B43" t="n">
         <v>0</v>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45852</v>
+        <v>45845</v>
       </c>
       <c r="B44" t="n">
         <v>12</v>
@@ -2096,7 +2096,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45853</v>
+        <v>45846</v>
       </c>
       <c r="B45" t="n">
         <v>12</v>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45854</v>
+        <v>45847</v>
       </c>
       <c r="B46" t="n">
         <v>12</v>
@@ -2138,7 +2138,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45855</v>
+        <v>45848</v>
       </c>
       <c r="B47" t="n">
         <v>12</v>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45856</v>
+        <v>45849</v>
       </c>
       <c r="B48" t="n">
         <v>12</v>
@@ -2180,7 +2180,7 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45857</v>
+        <v>45850</v>
       </c>
       <c r="B49" t="n">
         <v>0</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45858</v>
+        <v>45851</v>
       </c>
       <c r="B50" t="n">
         <v>0</v>
@@ -2226,7 +2226,7 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45859</v>
+        <v>45852</v>
       </c>
       <c r="B51" t="n">
         <v>12</v>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45860</v>
+        <v>45853</v>
       </c>
       <c r="B52" t="n">
         <v>12</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45861</v>
+        <v>45854</v>
       </c>
       <c r="B53" t="n">
         <v>12</v>
@@ -2289,7 +2289,7 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45862</v>
+        <v>45855</v>
       </c>
       <c r="B54" t="n">
         <v>12</v>
@@ -2310,7 +2310,7 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45863</v>
+        <v>45856</v>
       </c>
       <c r="B55" t="n">
         <v>12</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45864</v>
+        <v>45857</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45865</v>
+        <v>45858</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>45866</v>
+        <v>45859</v>
       </c>
       <c r="B58" t="n">
         <v>12</v>
@@ -2398,7 +2398,7 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>45867</v>
+        <v>45860</v>
       </c>
       <c r="B59" t="n">
         <v>12</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>45868</v>
+        <v>45861</v>
       </c>
       <c r="B60" t="n">
         <v>12</v>
@@ -2440,7 +2440,7 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>45869</v>
+        <v>45862</v>
       </c>
       <c r="B61" t="n">
         <v>12</v>
@@ -2461,7 +2461,7 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>45870</v>
+        <v>45863</v>
       </c>
       <c r="B62" t="n">
         <v>12</v>
@@ -2482,7 +2482,7 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>45871</v>
+        <v>45864</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
@@ -2505,7 +2505,7 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>45872</v>
+        <v>45865</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
@@ -2528,7 +2528,7 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>45873</v>
+        <v>45866</v>
       </c>
       <c r="B65" t="n">
         <v>12</v>
@@ -2549,7 +2549,7 @@
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>45874</v>
+        <v>45867</v>
       </c>
       <c r="B66" t="n">
         <v>12</v>
@@ -2570,7 +2570,7 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>45875</v>
+        <v>45868</v>
       </c>
       <c r="B67" t="n">
         <v>12</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>45876</v>
+        <v>45869</v>
       </c>
       <c r="B68" t="n">
         <v>12</v>
@@ -2612,7 +2612,7 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>45877</v>
+        <v>45870</v>
       </c>
       <c r="B69" t="n">
         <v>12</v>
@@ -2633,7 +2633,7 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>45878</v>
+        <v>45871</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
@@ -2656,7 +2656,7 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>45879</v>
+        <v>45872</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>45880</v>
+        <v>45873</v>
       </c>
       <c r="B72" t="n">
         <v>12</v>
@@ -2700,7 +2700,7 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>45881</v>
+        <v>45874</v>
       </c>
       <c r="B73" t="n">
         <v>12</v>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>45882</v>
+        <v>45875</v>
       </c>
       <c r="B74" t="n">
         <v>12</v>
@@ -2742,7 +2742,7 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>45883</v>
+        <v>45876</v>
       </c>
       <c r="B75" t="n">
         <v>12</v>
@@ -2763,7 +2763,7 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>45884</v>
+        <v>45877</v>
       </c>
       <c r="B76" t="n">
         <v>12</v>
@@ -2784,7 +2784,7 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>45885</v>
+        <v>45878</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
@@ -2807,7 +2807,7 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>45886</v>
+        <v>45879</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
@@ -2830,7 +2830,7 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>45887</v>
+        <v>45880</v>
       </c>
       <c r="B79" t="n">
         <v>12</v>
@@ -2851,7 +2851,7 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>45888</v>
+        <v>45881</v>
       </c>
       <c r="B80" t="n">
         <v>12</v>
@@ -2872,7 +2872,7 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>45889</v>
+        <v>45882</v>
       </c>
       <c r="B81" t="n">
         <v>12</v>
@@ -2893,7 +2893,7 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>45890</v>
+        <v>45883</v>
       </c>
       <c r="B82" t="n">
         <v>12</v>
@@ -2914,7 +2914,7 @@
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>45891</v>
+        <v>45884</v>
       </c>
       <c r="B83" t="n">
         <v>12</v>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>45892</v>
+        <v>45885</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
@@ -2958,7 +2958,7 @@
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>45893</v>
+        <v>45886</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
@@ -2981,7 +2981,7 @@
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>45894</v>
+        <v>45887</v>
       </c>
       <c r="B86" t="n">
         <v>12</v>
@@ -3002,7 +3002,7 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>45895</v>
+        <v>45888</v>
       </c>
       <c r="B87" t="n">
         <v>12</v>
@@ -3023,7 +3023,7 @@
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>45896</v>
+        <v>45889</v>
       </c>
       <c r="B88" t="n">
         <v>12</v>
@@ -3044,7 +3044,7 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>45897</v>
+        <v>45890</v>
       </c>
       <c r="B89" t="n">
         <v>12</v>
@@ -3065,7 +3065,7 @@
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>45898</v>
+        <v>45891</v>
       </c>
       <c r="B90" t="n">
         <v>12</v>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>45899</v>
+        <v>45892</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
@@ -3109,7 +3109,7 @@
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>45900</v>
+        <v>45893</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
@@ -3132,7 +3132,7 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>45901</v>
+        <v>45894</v>
       </c>
       <c r="B93" t="n">
         <v>12</v>
@@ -3153,7 +3153,7 @@
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>45902</v>
+        <v>45895</v>
       </c>
       <c r="B94" t="n">
         <v>12</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>45903</v>
+        <v>45896</v>
       </c>
       <c r="B95" t="n">
         <v>12</v>
@@ -3195,7 +3195,7 @@
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>45904</v>
+        <v>45897</v>
       </c>
       <c r="B96" t="n">
         <v>12</v>
@@ -3216,7 +3216,7 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>45905</v>
+        <v>45898</v>
       </c>
       <c r="B97" t="n">
         <v>12</v>
@@ -3237,7 +3237,7 @@
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>45906</v>
+        <v>45899</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>45907</v>
+        <v>45900</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
@@ -3283,7 +3283,7 @@
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>45908</v>
+        <v>45901</v>
       </c>
       <c r="B100" t="n">
         <v>12</v>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>45909</v>
+        <v>45902</v>
       </c>
       <c r="B101" t="n">
         <v>12</v>
@@ -3325,7 +3325,7 @@
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>45910</v>
+        <v>45903</v>
       </c>
       <c r="B102" t="n">
         <v>12</v>
@@ -3346,7 +3346,7 @@
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>45911</v>
+        <v>45904</v>
       </c>
       <c r="B103" t="n">
         <v>12</v>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>45912</v>
+        <v>45905</v>
       </c>
       <c r="B104" t="n">
         <v>12</v>
@@ -3388,7 +3388,7 @@
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>45913</v>
+        <v>45906</v>
       </c>
       <c r="B105" t="n">
         <v>0</v>
@@ -3411,7 +3411,7 @@
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>45914</v>
+        <v>45907</v>
       </c>
       <c r="B106" t="n">
         <v>0</v>
@@ -3434,7 +3434,7 @@
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>45915</v>
+        <v>45908</v>
       </c>
       <c r="B107" t="n">
         <v>12</v>
@@ -3455,7 +3455,7 @@
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>45916</v>
+        <v>45909</v>
       </c>
       <c r="B108" t="n">
         <v>12</v>
@@ -3476,7 +3476,7 @@
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>45917</v>
+        <v>45910</v>
       </c>
       <c r="B109" t="n">
         <v>12</v>
@@ -3497,7 +3497,7 @@
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>45918</v>
+        <v>45911</v>
       </c>
       <c r="B110" t="n">
         <v>12</v>
@@ -3518,7 +3518,7 @@
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>45919</v>
+        <v>45912</v>
       </c>
       <c r="B111" t="n">
         <v>12</v>
@@ -3539,7 +3539,7 @@
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>45920</v>
+        <v>45913</v>
       </c>
       <c r="B112" t="n">
         <v>0</v>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>45921</v>
+        <v>45914</v>
       </c>
       <c r="B113" t="n">
         <v>0</v>
@@ -3585,7 +3585,7 @@
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>45922</v>
+        <v>45915</v>
       </c>
       <c r="B114" t="n">
         <v>12</v>
@@ -3606,7 +3606,7 @@
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>45923</v>
+        <v>45916</v>
       </c>
       <c r="B115" t="n">
         <v>12</v>
@@ -3627,7 +3627,7 @@
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>45924</v>
+        <v>45917</v>
       </c>
       <c r="B116" t="n">
         <v>12</v>
@@ -3648,7 +3648,7 @@
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>45925</v>
+        <v>45918</v>
       </c>
       <c r="B117" t="n">
         <v>12</v>
@@ -3669,10 +3669,10 @@
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>45926</v>
+        <v>45919</v>
       </c>
       <c r="B118" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C118" t="n">
         <v>25</v>
@@ -3680,19 +3680,17 @@
       <c r="D118" t="n">
         <v>37.5</v>
       </c>
-      <c r="E118" t="n">
-        <v>40</v>
-      </c>
+      <c r="E118" t="inlineStr"/>
       <c r="F118" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G118" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>45927</v>
+        <v>45920</v>
       </c>
       <c r="B119" t="n">
         <v>0</v>
@@ -3715,7 +3713,7 @@
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>45928</v>
+        <v>45921</v>
       </c>
       <c r="B120" t="n">
         <v>0</v>
@@ -3738,7 +3736,7 @@
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>45929</v>
+        <v>45922</v>
       </c>
       <c r="B121" t="n">
         <v>12</v>
@@ -3759,7 +3757,7 @@
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>45930</v>
+        <v>45923</v>
       </c>
       <c r="B122" t="n">
         <v>12</v>
@@ -3780,7 +3778,7 @@
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>45931</v>
+        <v>45924</v>
       </c>
       <c r="B123" t="n">
         <v>12</v>
@@ -3801,7 +3799,7 @@
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>45932</v>
+        <v>45925</v>
       </c>
       <c r="B124" t="n">
         <v>12</v>
@@ -3822,10 +3820,10 @@
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>45933</v>
+        <v>45926</v>
       </c>
       <c r="B125" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C125" t="n">
         <v>25</v>
@@ -3833,17 +3831,19 @@
       <c r="D125" t="n">
         <v>37.5</v>
       </c>
-      <c r="E125" t="inlineStr"/>
+      <c r="E125" t="n">
+        <v>40</v>
+      </c>
       <c r="F125" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G125" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>45934</v>
+        <v>45927</v>
       </c>
       <c r="B126" t="n">
         <v>0</v>
@@ -3866,7 +3866,7 @@
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>45935</v>
+        <v>45928</v>
       </c>
       <c r="B127" t="n">
         <v>0</v>
@@ -3889,7 +3889,7 @@
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
-        <v>45936</v>
+        <v>45929</v>
       </c>
       <c r="B128" t="n">
         <v>12</v>
@@ -3910,7 +3910,7 @@
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
-        <v>45937</v>
+        <v>45930</v>
       </c>
       <c r="B129" t="n">
         <v>12</v>
@@ -3931,7 +3931,7 @@
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
-        <v>45938</v>
+        <v>45931</v>
       </c>
       <c r="B130" t="n">
         <v>12</v>
@@ -3952,7 +3952,7 @@
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
-        <v>45939</v>
+        <v>45932</v>
       </c>
       <c r="B131" t="n">
         <v>12</v>
@@ -3973,7 +3973,7 @@
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
-        <v>45940</v>
+        <v>45933</v>
       </c>
       <c r="B132" t="n">
         <v>12</v>
@@ -3994,7 +3994,7 @@
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
-        <v>45941</v>
+        <v>45934</v>
       </c>
       <c r="B133" t="n">
         <v>0</v>
@@ -4017,7 +4017,7 @@
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
-        <v>45942</v>
+        <v>45935</v>
       </c>
       <c r="B134" t="n">
         <v>0</v>
@@ -4040,7 +4040,7 @@
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
-        <v>45943</v>
+        <v>45936</v>
       </c>
       <c r="B135" t="n">
         <v>12</v>
@@ -4061,7 +4061,7 @@
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
-        <v>45944</v>
+        <v>45937</v>
       </c>
       <c r="B136" t="n">
         <v>12</v>
@@ -4082,7 +4082,7 @@
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
-        <v>45945</v>
+        <v>45938</v>
       </c>
       <c r="B137" t="n">
         <v>12</v>
@@ -4103,7 +4103,7 @@
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
-        <v>45946</v>
+        <v>45939</v>
       </c>
       <c r="B138" t="n">
         <v>12</v>
@@ -4124,7 +4124,7 @@
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
-        <v>45947</v>
+        <v>45940</v>
       </c>
       <c r="B139" t="n">
         <v>12</v>
@@ -4145,7 +4145,7 @@
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
-        <v>45948</v>
+        <v>45941</v>
       </c>
       <c r="B140" t="n">
         <v>0</v>
@@ -4168,7 +4168,7 @@
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
-        <v>45949</v>
+        <v>45942</v>
       </c>
       <c r="B141" t="n">
         <v>0</v>
@@ -4191,7 +4191,7 @@
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
-        <v>45950</v>
+        <v>45943</v>
       </c>
       <c r="B142" t="n">
         <v>12</v>
@@ -4212,7 +4212,7 @@
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
-        <v>45951</v>
+        <v>45944</v>
       </c>
       <c r="B143" t="n">
         <v>12</v>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
-        <v>45952</v>
+        <v>45945</v>
       </c>
       <c r="B144" t="n">
         <v>12</v>
@@ -4254,7 +4254,7 @@
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
-        <v>45953</v>
+        <v>45946</v>
       </c>
       <c r="B145" t="n">
         <v>12</v>
@@ -4275,7 +4275,7 @@
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
-        <v>45954</v>
+        <v>45947</v>
       </c>
       <c r="B146" t="n">
         <v>12</v>
@@ -4296,7 +4296,7 @@
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
-        <v>45955</v>
+        <v>45948</v>
       </c>
       <c r="B147" t="n">
         <v>0</v>
@@ -4319,7 +4319,7 @@
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
-        <v>45956</v>
+        <v>45949</v>
       </c>
       <c r="B148" t="n">
         <v>0</v>
@@ -4342,7 +4342,7 @@
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
-        <v>45957</v>
+        <v>45950</v>
       </c>
       <c r="B149" t="n">
         <v>12</v>
@@ -4363,7 +4363,7 @@
     </row>
     <row r="150">
       <c r="A150" s="2" t="n">
-        <v>45958</v>
+        <v>45951</v>
       </c>
       <c r="B150" t="n">
         <v>12</v>
@@ -4384,7 +4384,7 @@
     </row>
     <row r="151">
       <c r="A151" s="2" t="n">
-        <v>45959</v>
+        <v>45952</v>
       </c>
       <c r="B151" t="n">
         <v>12</v>
@@ -4405,7 +4405,7 @@
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
-        <v>45960</v>
+        <v>45953</v>
       </c>
       <c r="B152" t="n">
         <v>12</v>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="153">
       <c r="A153" s="2" t="n">
-        <v>45961</v>
+        <v>45954</v>
       </c>
       <c r="B153" t="n">
         <v>12</v>
@@ -4447,7 +4447,7 @@
     </row>
     <row r="154">
       <c r="A154" s="2" t="n">
-        <v>45962</v>
+        <v>45955</v>
       </c>
       <c r="B154" t="n">
         <v>0</v>
@@ -4470,7 +4470,7 @@
     </row>
     <row r="155">
       <c r="A155" s="2" t="n">
-        <v>45963</v>
+        <v>45956</v>
       </c>
       <c r="B155" t="n">
         <v>0</v>
@@ -4493,7 +4493,7 @@
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
-        <v>45964</v>
+        <v>45957</v>
       </c>
       <c r="B156" t="n">
         <v>12</v>
@@ -4514,10 +4514,10 @@
     </row>
     <row r="157">
       <c r="A157" s="2" t="n">
-        <v>45965</v>
+        <v>45958</v>
       </c>
       <c r="B157" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C157" t="n">
         <v>25</v>
@@ -4525,19 +4525,17 @@
       <c r="D157" t="n">
         <v>37.5</v>
       </c>
-      <c r="E157" t="n">
-        <v>40</v>
-      </c>
+      <c r="E157" t="inlineStr"/>
       <c r="F157" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G157" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="n">
-        <v>45966</v>
+        <v>45959</v>
       </c>
       <c r="B158" t="n">
         <v>12</v>
@@ -4558,7 +4556,7 @@
     </row>
     <row r="159">
       <c r="A159" s="2" t="n">
-        <v>45967</v>
+        <v>45960</v>
       </c>
       <c r="B159" t="n">
         <v>12</v>
@@ -4579,7 +4577,7 @@
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
-        <v>45968</v>
+        <v>45961</v>
       </c>
       <c r="B160" t="n">
         <v>12</v>
@@ -4600,7 +4598,7 @@
     </row>
     <row r="161">
       <c r="A161" s="2" t="n">
-        <v>45969</v>
+        <v>45962</v>
       </c>
       <c r="B161" t="n">
         <v>0</v>
@@ -4623,7 +4621,7 @@
     </row>
     <row r="162">
       <c r="A162" s="2" t="n">
-        <v>45970</v>
+        <v>45963</v>
       </c>
       <c r="B162" t="n">
         <v>0</v>
@@ -4646,7 +4644,7 @@
     </row>
     <row r="163">
       <c r="A163" s="2" t="n">
-        <v>45971</v>
+        <v>45964</v>
       </c>
       <c r="B163" t="n">
         <v>12</v>
@@ -4667,10 +4665,10 @@
     </row>
     <row r="164">
       <c r="A164" s="2" t="n">
-        <v>45972</v>
+        <v>45965</v>
       </c>
       <c r="B164" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C164" t="n">
         <v>25</v>
@@ -4678,17 +4676,19 @@
       <c r="D164" t="n">
         <v>37.5</v>
       </c>
-      <c r="E164" t="inlineStr"/>
+      <c r="E164" t="n">
+        <v>40</v>
+      </c>
       <c r="F164" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G164" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="2" t="n">
-        <v>45973</v>
+        <v>45966</v>
       </c>
       <c r="B165" t="n">
         <v>12</v>
@@ -4709,7 +4709,7 @@
     </row>
     <row r="166">
       <c r="A166" s="2" t="n">
-        <v>45974</v>
+        <v>45967</v>
       </c>
       <c r="B166" t="n">
         <v>12</v>
@@ -4730,7 +4730,7 @@
     </row>
     <row r="167">
       <c r="A167" s="2" t="n">
-        <v>45975</v>
+        <v>45968</v>
       </c>
       <c r="B167" t="n">
         <v>12</v>
@@ -4751,7 +4751,7 @@
     </row>
     <row r="168">
       <c r="A168" s="2" t="n">
-        <v>45976</v>
+        <v>45969</v>
       </c>
       <c r="B168" t="n">
         <v>0</v>
@@ -4774,7 +4774,7 @@
     </row>
     <row r="169">
       <c r="A169" s="2" t="n">
-        <v>45977</v>
+        <v>45970</v>
       </c>
       <c r="B169" t="n">
         <v>0</v>
@@ -4797,7 +4797,7 @@
     </row>
     <row r="170">
       <c r="A170" s="2" t="n">
-        <v>45978</v>
+        <v>45971</v>
       </c>
       <c r="B170" t="n">
         <v>12</v>
@@ -4818,7 +4818,7 @@
     </row>
     <row r="171">
       <c r="A171" s="2" t="n">
-        <v>45979</v>
+        <v>45972</v>
       </c>
       <c r="B171" t="n">
         <v>12</v>
@@ -4839,7 +4839,7 @@
     </row>
     <row r="172">
       <c r="A172" s="2" t="n">
-        <v>45980</v>
+        <v>45973</v>
       </c>
       <c r="B172" t="n">
         <v>12</v>
@@ -4860,7 +4860,7 @@
     </row>
     <row r="173">
       <c r="A173" s="2" t="n">
-        <v>45981</v>
+        <v>45974</v>
       </c>
       <c r="B173" t="n">
         <v>12</v>
@@ -4881,7 +4881,7 @@
     </row>
     <row r="174">
       <c r="A174" s="2" t="n">
-        <v>45982</v>
+        <v>45975</v>
       </c>
       <c r="B174" t="n">
         <v>12</v>
@@ -4902,7 +4902,7 @@
     </row>
     <row r="175">
       <c r="A175" s="2" t="n">
-        <v>45983</v>
+        <v>45976</v>
       </c>
       <c r="B175" t="n">
         <v>0</v>
@@ -4925,7 +4925,7 @@
     </row>
     <row r="176">
       <c r="A176" s="2" t="n">
-        <v>45984</v>
+        <v>45977</v>
       </c>
       <c r="B176" t="n">
         <v>0</v>
@@ -4948,7 +4948,7 @@
     </row>
     <row r="177">
       <c r="A177" s="2" t="n">
-        <v>45985</v>
+        <v>45978</v>
       </c>
       <c r="B177" t="n">
         <v>12</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="178">
       <c r="A178" s="2" t="n">
-        <v>45986</v>
+        <v>45979</v>
       </c>
       <c r="B178" t="n">
         <v>12</v>
@@ -4990,7 +4990,7 @@
     </row>
     <row r="179">
       <c r="A179" s="2" t="n">
-        <v>45987</v>
+        <v>45980</v>
       </c>
       <c r="B179" t="n">
         <v>12</v>
@@ -5011,7 +5011,7 @@
     </row>
     <row r="180">
       <c r="A180" s="2" t="n">
-        <v>45988</v>
+        <v>45981</v>
       </c>
       <c r="B180" t="n">
         <v>12</v>
@@ -5032,7 +5032,7 @@
     </row>
     <row r="181">
       <c r="A181" s="2" t="n">
-        <v>45989</v>
+        <v>45982</v>
       </c>
       <c r="B181" t="n">
         <v>12</v>
@@ -5053,7 +5053,7 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45990</v>
+        <v>45983</v>
       </c>
       <c r="B182" t="n">
         <v>0</v>
@@ -5076,7 +5076,7 @@
     </row>
     <row r="183">
       <c r="A183" s="2" t="n">
-        <v>45991</v>
+        <v>45984</v>
       </c>
       <c r="B183" t="n">
         <v>0</v>
@@ -5099,7 +5099,7 @@
     </row>
     <row r="184">
       <c r="A184" s="2" t="n">
-        <v>45992</v>
+        <v>45985</v>
       </c>
       <c r="B184" t="n">
         <v>12</v>
@@ -5120,7 +5120,7 @@
     </row>
     <row r="185">
       <c r="A185" s="2" t="n">
-        <v>45993</v>
+        <v>45986</v>
       </c>
       <c r="B185" t="n">
         <v>12</v>
@@ -5141,7 +5141,7 @@
     </row>
     <row r="186">
       <c r="A186" s="2" t="n">
-        <v>45994</v>
+        <v>45987</v>
       </c>
       <c r="B186" t="n">
         <v>12</v>
@@ -5162,7 +5162,7 @@
     </row>
     <row r="187">
       <c r="A187" s="2" t="n">
-        <v>45995</v>
+        <v>45988</v>
       </c>
       <c r="B187" t="n">
         <v>12</v>
@@ -5183,7 +5183,7 @@
     </row>
     <row r="188">
       <c r="A188" s="2" t="n">
-        <v>45996</v>
+        <v>45989</v>
       </c>
       <c r="B188" t="n">
         <v>12</v>
@@ -5204,7 +5204,7 @@
     </row>
     <row r="189">
       <c r="A189" s="2" t="n">
-        <v>45997</v>
+        <v>45990</v>
       </c>
       <c r="B189" t="n">
         <v>0</v>
@@ -5227,7 +5227,7 @@
     </row>
     <row r="190">
       <c r="A190" s="2" t="n">
-        <v>45998</v>
+        <v>45991</v>
       </c>
       <c r="B190" t="n">
         <v>0</v>
@@ -5250,7 +5250,7 @@
     </row>
     <row r="191">
       <c r="A191" s="2" t="n">
-        <v>45999</v>
+        <v>45992</v>
       </c>
       <c r="B191" t="n">
         <v>12</v>
@@ -5271,7 +5271,7 @@
     </row>
     <row r="192">
       <c r="A192" s="2" t="n">
-        <v>46000</v>
+        <v>45993</v>
       </c>
       <c r="B192" t="n">
         <v>12</v>
@@ -5292,7 +5292,7 @@
     </row>
     <row r="193">
       <c r="A193" s="2" t="n">
-        <v>46001</v>
+        <v>45994</v>
       </c>
       <c r="B193" t="n">
         <v>12</v>
@@ -5313,7 +5313,7 @@
     </row>
     <row r="194">
       <c r="A194" s="2" t="n">
-        <v>46002</v>
+        <v>45995</v>
       </c>
       <c r="B194" t="n">
         <v>12</v>
@@ -5334,7 +5334,7 @@
     </row>
     <row r="195">
       <c r="A195" s="2" t="n">
-        <v>46003</v>
+        <v>45996</v>
       </c>
       <c r="B195" t="n">
         <v>12</v>
@@ -5355,7 +5355,7 @@
     </row>
     <row r="196">
       <c r="A196" s="2" t="n">
-        <v>46004</v>
+        <v>45997</v>
       </c>
       <c r="B196" t="n">
         <v>0</v>
@@ -5378,7 +5378,7 @@
     </row>
     <row r="197">
       <c r="A197" s="2" t="n">
-        <v>46005</v>
+        <v>45998</v>
       </c>
       <c r="B197" t="n">
         <v>0</v>
@@ -5401,7 +5401,7 @@
     </row>
     <row r="198">
       <c r="A198" s="2" t="n">
-        <v>46006</v>
+        <v>45999</v>
       </c>
       <c r="B198" t="n">
         <v>12</v>
@@ -5422,7 +5422,7 @@
     </row>
     <row r="199">
       <c r="A199" s="2" t="n">
-        <v>46007</v>
+        <v>46000</v>
       </c>
       <c r="B199" t="n">
         <v>12</v>
@@ -5443,7 +5443,7 @@
     </row>
     <row r="200">
       <c r="A200" s="2" t="n">
-        <v>46008</v>
+        <v>46001</v>
       </c>
       <c r="B200" t="n">
         <v>12</v>
@@ -5464,7 +5464,7 @@
     </row>
     <row r="201">
       <c r="A201" s="2" t="n">
-        <v>46009</v>
+        <v>46002</v>
       </c>
       <c r="B201" t="n">
         <v>12</v>
@@ -5485,7 +5485,7 @@
     </row>
     <row r="202">
       <c r="A202" s="2" t="n">
-        <v>46010</v>
+        <v>46003</v>
       </c>
       <c r="B202" t="n">
         <v>12</v>
@@ -5506,7 +5506,7 @@
     </row>
     <row r="203">
       <c r="A203" s="2" t="n">
-        <v>46011</v>
+        <v>46004</v>
       </c>
       <c r="B203" t="n">
         <v>0</v>
@@ -5529,7 +5529,7 @@
     </row>
     <row r="204">
       <c r="A204" s="2" t="n">
-        <v>46012</v>
+        <v>46005</v>
       </c>
       <c r="B204" t="n">
         <v>0</v>
@@ -5552,7 +5552,7 @@
     </row>
     <row r="205">
       <c r="A205" s="2" t="n">
-        <v>46013</v>
+        <v>46006</v>
       </c>
       <c r="B205" t="n">
         <v>12</v>
@@ -5568,6 +5568,157 @@
         <v>0</v>
       </c>
       <c r="G205" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="2" t="n">
+        <v>46007</v>
+      </c>
+      <c r="B206" t="n">
+        <v>12</v>
+      </c>
+      <c r="C206" t="n">
+        <v>25</v>
+      </c>
+      <c r="D206" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="E206" t="inlineStr"/>
+      <c r="F206" t="n">
+        <v>0</v>
+      </c>
+      <c r="G206" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="2" t="n">
+        <v>46008</v>
+      </c>
+      <c r="B207" t="n">
+        <v>12</v>
+      </c>
+      <c r="C207" t="n">
+        <v>25</v>
+      </c>
+      <c r="D207" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="E207" t="inlineStr"/>
+      <c r="F207" t="n">
+        <v>0</v>
+      </c>
+      <c r="G207" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="2" t="n">
+        <v>46009</v>
+      </c>
+      <c r="B208" t="n">
+        <v>12</v>
+      </c>
+      <c r="C208" t="n">
+        <v>25</v>
+      </c>
+      <c r="D208" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="E208" t="inlineStr"/>
+      <c r="F208" t="n">
+        <v>0</v>
+      </c>
+      <c r="G208" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="2" t="n">
+        <v>46010</v>
+      </c>
+      <c r="B209" t="n">
+        <v>12</v>
+      </c>
+      <c r="C209" t="n">
+        <v>25</v>
+      </c>
+      <c r="D209" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="E209" t="inlineStr"/>
+      <c r="F209" t="n">
+        <v>0</v>
+      </c>
+      <c r="G209" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="2" t="n">
+        <v>46011</v>
+      </c>
+      <c r="B210" t="n">
+        <v>0</v>
+      </c>
+      <c r="C210" t="n">
+        <v>25</v>
+      </c>
+      <c r="D210" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="E210" t="n">
+        <v>40</v>
+      </c>
+      <c r="F210" t="n">
+        <v>4</v>
+      </c>
+      <c r="G210" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="2" t="n">
+        <v>46012</v>
+      </c>
+      <c r="B211" t="n">
+        <v>0</v>
+      </c>
+      <c r="C211" t="n">
+        <v>25</v>
+      </c>
+      <c r="D211" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="E211" t="n">
+        <v>40</v>
+      </c>
+      <c r="F211" t="n">
+        <v>4</v>
+      </c>
+      <c r="G211" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="2" t="n">
+        <v>46013</v>
+      </c>
+      <c r="B212" t="n">
+        <v>12</v>
+      </c>
+      <c r="C212" t="n">
+        <v>25</v>
+      </c>
+      <c r="D212" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="E212" t="inlineStr"/>
+      <c r="F212" t="n">
+        <v>0</v>
+      </c>
+      <c r="G212" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: Add missing day_of_week values to truck schedules
Added missing day_of_week values in Network_Config.xlsx TruckSchedules sheet:
- T1: monday
- T2: tuesday
- T4: thursday
- T5: friday

Previously these trucks had NULL day_of_week values, causing them to run
EVERY day instead of their scheduled day. This resulted in daily truck
departures from manufacturing (6122) instead of the intended Mon-Fri
day-specific schedule.

With this fix:
- T1 runs Monday only
- T2 runs Tuesday only
- T3 runs Wednesday only (already correct)
- T4 runs Thursday only
- T5 runs Friday only

This ensures proper truck schedule adherence and prevents over-utilization
of manufacturing capacity.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/examples/Network_Config.xlsx
+++ b/data/examples/Network_Config.xlsx
@@ -563,7 +563,6 @@
           <t>ambient</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
         <v>50000</v>
       </c>
@@ -589,7 +588,6 @@
           <t>ambient</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
         <v>50000</v>
       </c>
@@ -615,7 +613,6 @@
           <t>ambient</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
         <v>30000</v>
       </c>
@@ -641,7 +638,6 @@
           <t>ambient</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
         <v>15000</v>
       </c>
@@ -667,7 +663,6 @@
           <t>ambient</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
         <v>35000</v>
       </c>
@@ -693,7 +688,6 @@
           <t>ambient</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
         <v>25000</v>
       </c>
@@ -719,7 +713,6 @@
           <t>both</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
         <v>10000</v>
       </c>
@@ -745,7 +738,6 @@
           <t>ambient</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
         <v>40000</v>
       </c>
@@ -771,7 +763,6 @@
           <t>both</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
         <v>15000</v>
       </c>
@@ -797,7 +788,6 @@
           <t>both</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
         <v>50000</v>
       </c>
@@ -13589,6 +13579,11 @@
       <c r="H2" t="n">
         <v>0.3</v>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>monday</t>
+        </is>
+      </c>
       <c r="K2" t="n">
         <v>44</v>
       </c>
@@ -13632,6 +13627,11 @@
       <c r="H3" t="n">
         <v>0.3</v>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>tuesday</t>
+        </is>
+      </c>
       <c r="K3" t="n">
         <v>44</v>
       </c>
@@ -13728,6 +13728,11 @@
       <c r="H5" t="n">
         <v>0.3</v>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>thursday</t>
+        </is>
+      </c>
       <c r="K5" t="n">
         <v>44</v>
       </c>
@@ -13770,6 +13775,11 @@
       </c>
       <c r="H6" t="n">
         <v>0.3</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>friday</t>
+        </is>
       </c>
       <c r="K6" t="n">
         <v>44</v>

</xml_diff>

<commit_message>
Fix: Update 6122 and Lineage storage modes (ambient and frozen)
Complete storage_mode simplification in Network_Config.xlsx.

CHANGES:
========
- 6122 (Manufacturing): both → ambient (produces fresh product)
- Lineage (Frozen Storage): both → frozen (frozen storage only)

ALL NODES NOW:
==============
- 6122: ambient (manufacturing)
- 6104, 6105, 6103, 6110, 6123, 6125: ambient (hubs/spokes)
- 6120, 6130: ambient (breadrooms)
- Lineage: frozen (frozen buffer for WA)

No more 'both' anywhere - all nodes frozen OR ambient only!

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/examples/Network_Config.xlsx
+++ b/data/examples/Network_Config.xlsx
@@ -532,7 +532,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>both</t>
+          <t>ambient</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -785,7 +785,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>both</t>
+          <t>frozen</t>
         </is>
       </c>
       <c r="F12" t="n">

</xml_diff>